<commit_message>
9/19/2024 - Final Admin Mangement System
</commit_message>
<xml_diff>
--- a/NewVendorInfo.xlsx
+++ b/NewVendorInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesus\Desktop\WinFormsApp-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{098B1631-DBCF-4CB3-A5DD-23E6CD28616E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8030401-8723-45D6-A63D-C607E00CEB3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="690" windowWidth="26655" windowHeight="11295" xr2:uid="{4CE66CE1-6A7C-42A1-8B7C-F2B66E025779}"/>
+    <workbookView xWindow="0" yWindow="1485" windowWidth="26655" windowHeight="11295" xr2:uid="{4CE66CE1-6A7C-42A1-8B7C-F2B66E025779}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>POC_Name</t>
   </si>
@@ -60,6 +60,27 @@
   </si>
   <si>
     <t>POC_CompanyAddress</t>
+  </si>
+  <si>
+    <t>Jesus</t>
+  </si>
+  <si>
+    <t>Project Manager</t>
+  </si>
+  <si>
+    <t>jbusti@ksu.edu</t>
+  </si>
+  <si>
+    <t>(555) 555-5555</t>
+  </si>
+  <si>
+    <t>Bear's in the Forest</t>
+  </si>
+  <si>
+    <t>Bears@forest.gov</t>
+  </si>
+  <si>
+    <t>Manhattan</t>
   </si>
 </sst>
 </file>
@@ -112,6 +133,61 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7AC95437-3000-A0A3-9FF3-5A3EFD781AAF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7734300" y="190500"/>
+          <a:ext cx="190500" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -431,22 +507,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BA50AE4-ADF3-495E-8092-4EB95D1FC98D}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -475,7 +551,31 @@
         <v>6</v>
       </c>
     </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>